<commit_message>
added reference mesurement results
</commit_message>
<xml_diff>
--- a/experiments/11_sched_method_comparison_6/temperatures_a.xlsx
+++ b/experiments/11_sched_method_comparison_6/temperatures_a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\DP\experiments\11_sched_method_comparison_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E5CC4A-2C3D-4AA1-9E92-90ABFBD2A3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14218C0A-EE8B-4E93-8A38-9FA1B2977675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D9B2736F-8484-4142-882C-94BEA7D2BB42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D9B2736F-8484-4142-882C-94BEA7D2BB42}"/>
   </bookViews>
   <sheets>
     <sheet name="imx8 results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
   <si>
     <t>Run 1</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>Min util LTF</t>
+  </si>
+  <si>
+    <t>Mod.2 B predictor(2)</t>
+  </si>
+  <si>
+    <t>Mod.2 B predictor(2) LTF</t>
+  </si>
+  <si>
+    <t>ilp reference</t>
+  </si>
+  <si>
+    <t>reference</t>
   </si>
 </sst>
 </file>
@@ -1105,6 +1117,9 @@
               <c:f>'imx8 results'!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor(2)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1129,13 +1144,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.0287636592855831</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.118772343041941</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0349119125155843</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1147,13 +1162,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.0287636592855831</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.118772343041941</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0349119125155843</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1196,13 +1211,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>53.426000000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>54.093333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53.362000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1221,6 +1236,9 @@
               <c:f>'imx8 results'!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor(2) LTF</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1247,13 +1265,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.99692505011939325</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.1224085213899995</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0462134900041526</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1265,13 +1283,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.99692505011939325</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.1224085213899995</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0462134900041526</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1314,13 +1332,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>53.922666666666665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>54.206666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53.506</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1339,6 +1357,9 @@
               <c:f>'imx8 results'!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ilp reference</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1365,13 +1386,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.0613417085096686</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.0309969285437601</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0082451201083096</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1383,13 +1404,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.0613417085096686</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.0309969285437601</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>1.0082451201083096</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1432,13 +1453,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>54.962666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>55.783999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>54.162666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1457,6 +1478,9 @@
               <c:f>'imx8 results'!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>reference</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1483,13 +1507,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.1346200538800071</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.0379072962242595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.79795962025378042</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1501,13 +1525,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>1.1346200538800071</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.0379072962242595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.79795962025378042</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1550,13 +1574,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>54.118000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>54.514666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>54.569333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2647,6 +2671,9 @@
               <c:f>'imx8 results'!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor(2)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2671,13 +2698,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.4725619630153135</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.42997637144382678</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.57631080349254449</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2689,13 +2716,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.4725619630153135</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.42997637144382678</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.57631080349254449</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2738,13 +2765,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>29.469466666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30.201800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>29.486933333333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2763,6 +2790,9 @@
               <c:f>'imx8 results'!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor(2) LTF</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2789,13 +2819,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.35229065020551154</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.46578590217678667</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.621734570018042</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2807,13 +2837,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.35229065020551154</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.46578590217678667</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.621734570018042</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2856,13 +2886,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>30.001733333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30.300200000000032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>29.6208666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2881,6 +2911,9 @@
               <c:f>'imx8 results'!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ilp reference</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2907,13 +2940,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.4235661407095172</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.40765561718467935</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.6635378780111354</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2925,13 +2958,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.4235661407095172</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.40765561718467935</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.6635378780111354</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2974,13 +3007,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>31.081666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31.865933333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>30.225466666666701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2999,6 +3032,9 @@
               <c:f>'imx8 results'!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>reference</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3025,13 +3061,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.46278498967303283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.4800315082251505</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.50887935265203676</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3043,13 +3079,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.46278498967303283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.4800315082251505</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.50887935265203676</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3092,13 +3128,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>30.209199999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30.632333333333403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>30.601266666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4974,8 +5010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C717F6D4-64AC-45FC-95B6-DC01725ED549}">
   <dimension ref="A35:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55:N55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5313,152 +5349,208 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="17" t="e">
+      <c r="A43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="3">
+        <v>54.787999999999997</v>
+      </c>
+      <c r="C43" s="3">
+        <v>52.302</v>
+      </c>
+      <c r="D43" s="3">
+        <v>53.188000000000002</v>
+      </c>
+      <c r="E43" s="17">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="17" t="e">
+        <v>53.426000000000009</v>
+      </c>
+      <c r="F43" s="17">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.0287636592855831</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.129999999999995</v>
       </c>
       <c r="H43" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.2272</v>
       </c>
       <c r="I43" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>29.051200000000001</v>
       </c>
       <c r="J43" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>29.469466666666666</v>
       </c>
       <c r="K43" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="21"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="22"/>
+        <v>0.4725619630153135</v>
+      </c>
+      <c r="L43" s="21">
+        <v>24.658000000000001</v>
+      </c>
+      <c r="M43" s="3">
+        <v>23.0748</v>
+      </c>
+      <c r="N43" s="22">
+        <v>24.136800000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="17" t="e">
+      <c r="A44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="3">
+        <v>55.22</v>
+      </c>
+      <c r="C44" s="3">
+        <v>52.795999999999999</v>
+      </c>
+      <c r="D44" s="3">
+        <v>53.752000000000002</v>
+      </c>
+      <c r="E44" s="17">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F44" s="17" t="e">
+        <v>53.922666666666665</v>
+      </c>
+      <c r="F44" s="17">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.99692505011939325</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.4998</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.7422</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>29.763200000000001</v>
       </c>
       <c r="J44" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30.001733333333334</v>
       </c>
       <c r="K44" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="21"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="22"/>
+        <v>0.35229065020551154</v>
+      </c>
+      <c r="L44" s="21">
+        <v>24.720199999999998</v>
+      </c>
+      <c r="M44" s="3">
+        <v>23.053799999999999</v>
+      </c>
+      <c r="N44" s="22">
+        <v>23.988800000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="17" t="e">
+      <c r="A45" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="3">
+        <v>56.411999999999999</v>
+      </c>
+      <c r="C45" s="3">
+        <v>53.9</v>
+      </c>
+      <c r="D45" s="3">
+        <v>54.576000000000001</v>
+      </c>
+      <c r="E45" s="17">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45" s="17" t="e">
+        <v>54.962666666666671</v>
+      </c>
+      <c r="F45" s="17">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.0613417085096686</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31.676399999999997</v>
       </c>
       <c r="H45" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30.8462</v>
       </c>
       <c r="I45" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30.7224</v>
       </c>
       <c r="J45" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>31.081666666666667</v>
       </c>
       <c r="K45" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="21"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="22"/>
+        <v>0.4235661407095172</v>
+      </c>
+      <c r="L45" s="21">
+        <v>24.735600000000002</v>
+      </c>
+      <c r="M45" s="3">
+        <v>23.053799999999999</v>
+      </c>
+      <c r="N45" s="22">
+        <v>23.8536</v>
+      </c>
     </row>
     <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="17" t="e">
+      <c r="A46" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="3">
+        <v>55.688000000000002</v>
+      </c>
+      <c r="C46" s="3">
+        <v>53.045999999999999</v>
+      </c>
+      <c r="D46" s="3">
+        <v>53.62</v>
+      </c>
+      <c r="E46" s="17">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" s="17" t="e">
+        <v>54.118000000000002</v>
+      </c>
+      <c r="F46" s="17">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.1346200538800071</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.862600000000004</v>
       </c>
       <c r="H46" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.914999999999999</v>
       </c>
       <c r="I46" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>29.849999999999998</v>
       </c>
       <c r="J46" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30.209199999999999</v>
       </c>
       <c r="K46" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L46" s="21"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="22"/>
+        <v>0.46278498967303283</v>
+      </c>
+      <c r="L46" s="21">
+        <v>24.825399999999998</v>
+      </c>
+      <c r="M46" s="3">
+        <v>23.131</v>
+      </c>
+      <c r="N46" s="22">
+        <v>23.77</v>
+      </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
@@ -5822,152 +5914,208 @@
       </c>
     </row>
     <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="17" t="e">
+      <c r="A57" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="3">
+        <v>55.607999999999997</v>
+      </c>
+      <c r="C57" s="3">
+        <v>52.94</v>
+      </c>
+      <c r="D57" s="3">
+        <v>53.731999999999999</v>
+      </c>
+      <c r="E57" s="17">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F57" s="17" t="e">
+        <v>54.093333333333334</v>
+      </c>
+      <c r="F57" s="17">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.118772343041941</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>30.790999999999997</v>
       </c>
       <c r="H57" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>29.776999999999997</v>
       </c>
       <c r="I57" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>30.037399999999998</v>
       </c>
       <c r="J57" s="17">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>30.201800000000002</v>
       </c>
       <c r="K57" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L57" s="21"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="22"/>
+        <v>0.42997637144382678</v>
+      </c>
+      <c r="L57" s="21">
+        <v>24.817</v>
+      </c>
+      <c r="M57" s="3">
+        <v>23.163</v>
+      </c>
+      <c r="N57" s="22">
+        <v>23.694600000000001</v>
+      </c>
     </row>
     <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="17" t="e">
+      <c r="A58" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="3">
+        <v>55.783999999999999</v>
+      </c>
+      <c r="C58" s="3">
+        <v>53.264000000000003</v>
+      </c>
+      <c r="D58" s="3">
+        <v>53.572000000000003</v>
+      </c>
+      <c r="E58" s="17">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58" s="17" t="e">
+        <v>54.206666666666671</v>
+      </c>
+      <c r="F58" s="17">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.1224085213899995</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>30.958600000000001</v>
       </c>
       <c r="H58" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>29.953200000000102</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>29.988800000000001</v>
       </c>
       <c r="J58" s="17">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>30.300200000000032</v>
       </c>
       <c r="K58" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L58" s="21"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="22"/>
+        <v>0.46578590217678667</v>
+      </c>
+      <c r="L58" s="21">
+        <v>24.825399999999998</v>
+      </c>
+      <c r="M58" s="3">
+        <v>23.310799999999901</v>
+      </c>
+      <c r="N58" s="22">
+        <v>23.583200000000001</v>
+      </c>
     </row>
     <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="17" t="e">
+      <c r="A59" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="3">
+        <v>57.231999999999999</v>
+      </c>
+      <c r="C59" s="3">
+        <v>54.911999999999999</v>
+      </c>
+      <c r="D59" s="3">
+        <v>55.207999999999998</v>
+      </c>
+      <c r="E59" s="17">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F59" s="17" t="e">
+        <v>55.783999999999999</v>
+      </c>
+      <c r="F59" s="17">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.0309969285437601</v>
       </c>
       <c r="G59" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>32.436799999999998</v>
       </c>
       <c r="H59" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>31.5108</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>31.650199999999998</v>
       </c>
       <c r="J59" s="17">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>31.865933333333331</v>
       </c>
       <c r="K59" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L59" s="21"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="22"/>
+        <v>0.40765561718467935</v>
+      </c>
+      <c r="L59" s="21">
+        <v>24.795200000000001</v>
+      </c>
+      <c r="M59" s="3">
+        <v>23.401199999999999</v>
+      </c>
+      <c r="N59" s="22">
+        <v>23.5578</v>
+      </c>
     </row>
     <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="17" t="e">
+      <c r="A60" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="3">
+        <v>55.98</v>
+      </c>
+      <c r="C60" s="3">
+        <v>53.856000000000002</v>
+      </c>
+      <c r="D60" s="3">
+        <v>53.707999999999998</v>
+      </c>
+      <c r="E60" s="17">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F60" s="17" t="e">
+        <v>54.514666666666663</v>
+      </c>
+      <c r="F60" s="17">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.0379072962242595</v>
       </c>
       <c r="G60" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>31.309200000000097</v>
       </c>
       <c r="H60" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>30.339000000000102</v>
       </c>
       <c r="I60" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>30.248799999999999</v>
       </c>
       <c r="J60" s="17">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>30.632333333333403</v>
       </c>
       <c r="K60" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L60" s="21"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="22"/>
+        <v>0.4800315082251505</v>
+      </c>
+      <c r="L60" s="21">
+        <v>24.6707999999999</v>
+      </c>
+      <c r="M60" s="3">
+        <v>23.5169999999999</v>
+      </c>
+      <c r="N60" s="22">
+        <v>23.459199999999999</v>
+      </c>
     </row>
     <row r="61" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
@@ -6331,152 +6479,208 @@
       </c>
     </row>
     <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="17" t="e">
+      <c r="A71" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" s="3">
+        <v>54.823999999999998</v>
+      </c>
+      <c r="C71" s="3">
+        <v>52.69</v>
+      </c>
+      <c r="D71" s="3">
+        <v>52.572000000000003</v>
+      </c>
+      <c r="E71" s="17">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F71" s="17" t="e">
+        <v>53.362000000000002</v>
+      </c>
+      <c r="F71" s="17">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.0349119125155843</v>
       </c>
       <c r="G71" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>30.298999999999999</v>
       </c>
       <c r="H71" s="3">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>29.020799999999998</v>
       </c>
       <c r="I71" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>29.141000000000002</v>
       </c>
       <c r="J71" s="17">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>29.486933333333337</v>
       </c>
       <c r="K71" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L71" s="21"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="22"/>
+        <v>0.57631080349254449</v>
+      </c>
+      <c r="L71" s="21">
+        <v>24.524999999999999</v>
+      </c>
+      <c r="M71" s="3">
+        <v>23.6692</v>
+      </c>
+      <c r="N71" s="22">
+        <v>23.431000000000001</v>
+      </c>
     </row>
     <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="17" t="e">
+      <c r="A72" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="3">
+        <v>54.984000000000002</v>
+      </c>
+      <c r="C72" s="3">
+        <v>52.826000000000001</v>
+      </c>
+      <c r="D72" s="3">
+        <v>52.707999999999998</v>
+      </c>
+      <c r="E72" s="17">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F72" s="17" t="e">
+        <v>53.506</v>
+      </c>
+      <c r="F72" s="17">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.0462134900041526</v>
       </c>
       <c r="G72" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>30.486800000000002</v>
       </c>
       <c r="H72" s="3">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>29.055800000000101</v>
       </c>
       <c r="I72" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>29.319999999999997</v>
       </c>
       <c r="J72" s="17">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>29.6208666666667</v>
       </c>
       <c r="K72" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L72" s="21"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="22"/>
+        <v>0.621734570018042</v>
+      </c>
+      <c r="L72" s="21">
+        <v>24.497199999999999</v>
+      </c>
+      <c r="M72" s="3">
+        <v>23.7701999999999</v>
+      </c>
+      <c r="N72" s="22">
+        <v>23.388000000000002</v>
+      </c>
     </row>
     <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="17" t="e">
+      <c r="A73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="3">
+        <v>55.527999999999999</v>
+      </c>
+      <c r="C73" s="3">
+        <v>53.835999999999999</v>
+      </c>
+      <c r="D73" s="3">
+        <v>53.124000000000002</v>
+      </c>
+      <c r="E73" s="17">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F73" s="17" t="e">
+        <v>54.162666666666667</v>
+      </c>
+      <c r="F73" s="17">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>1.0082451201083096</v>
       </c>
       <c r="G73" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>31.161799999999999</v>
       </c>
       <c r="H73" s="3">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>29.703600000000097</v>
       </c>
       <c r="I73" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>29.811000000000003</v>
       </c>
       <c r="J73" s="17">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>30.225466666666701</v>
       </c>
       <c r="K73" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L73" s="21"/>
-      <c r="M73" s="3"/>
-      <c r="N73" s="22"/>
+        <v>0.6635378780111354</v>
+      </c>
+      <c r="L73" s="21">
+        <v>24.366199999999999</v>
+      </c>
+      <c r="M73" s="3">
+        <v>24.132399999999901</v>
+      </c>
+      <c r="N73" s="22">
+        <v>23.312999999999999</v>
+      </c>
     </row>
     <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="17" t="e">
+      <c r="A74" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="3">
+        <v>55.6</v>
+      </c>
+      <c r="C74" s="3">
+        <v>54.451999999999998</v>
+      </c>
+      <c r="D74" s="3">
+        <v>53.655999999999999</v>
+      </c>
+      <c r="E74" s="17">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F74" s="17" t="e">
+        <v>54.569333333333333</v>
+      </c>
+      <c r="F74" s="17">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>0.79795962025378042</v>
       </c>
       <c r="G74" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>31.2956</v>
       </c>
       <c r="H74" s="3">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>30.090199999999999</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>30.417999999999999</v>
       </c>
       <c r="J74" s="17">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>30.601266666666664</v>
       </c>
       <c r="K74" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L74" s="21"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="22"/>
+        <v>0.50887935265203676</v>
+      </c>
+      <c r="L74" s="21">
+        <v>24.304400000000001</v>
+      </c>
+      <c r="M74" s="3">
+        <v>24.361799999999999</v>
+      </c>
+      <c r="N74" s="22">
+        <v>23.238</v>
+      </c>
     </row>
     <row r="75" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>

</xml_diff>